<commit_message>
update on LMER models and shamChange as a variable
</commit_message>
<xml_diff>
--- a/experiment-data/kiwiQuantReports.xlsx
+++ b/experiment-data/kiwiQuantReports.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hendrik/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hendrik/git/AAU/bci-kiwi-runner/experiment-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCBACB-1A19-2143-A973-70ECE2A55A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB1CDD-9E3C-4942-A6EB-81F43A08D456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="32220" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="kiwiGame" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">kiwiGame!$A$1:$L$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">kiwiGame!$A$1:$M$61</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="15">
   <si>
     <t>Timestamp</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>shamRate</t>
+  </si>
+  <si>
+    <t>shamChange</t>
   </si>
 </sst>
 </file>
@@ -522,30 +525,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="21.5" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,34 +559,37 @@
         <v>13</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="L1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="M1" s="30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>43633.398583738424</v>
       </c>
@@ -593,17 +599,18 @@
       <c r="C2" s="6">
         <v>15</v>
       </c>
-      <c r="D2" s="6">
-        <v>1</v>
+      <c r="D2" s="8" t="str">
+        <f>IF(E1=E2,IF(C2&lt;C1,-1,1),"")</f>
+        <v/>
       </c>
       <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
         <v>22</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="6">
-        <v>2</v>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H2" s="6">
         <v>2</v>
@@ -612,16 +619,19 @@
         <v>2</v>
       </c>
       <c r="J2" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L2" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M2" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
         <v>43633.402496377312</v>
       </c>
@@ -632,34 +642,38 @@
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>1</v>
+        <f>IF(E2=E3,IF(C3&lt;C2,-1,1),"")</f>
+        <v>-1</v>
       </c>
       <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
         <v>22</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="8">
-        <v>4</v>
+      <c r="G3" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="H3" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="8">
         <v>3</v>
       </c>
       <c r="L3" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>43633.406576967594</v>
       </c>
@@ -669,17 +683,18 @@
       <c r="C4" s="6">
         <v>30</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="8">
+        <f t="shared" ref="D4:D61" si="0">IF(E3=E4,IF(C4&lt;C3,-1,1),"")</f>
         <v>1</v>
       </c>
       <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
         <v>22</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6">
-        <v>4</v>
+      <c r="G4" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H4" s="6">
         <v>4</v>
@@ -688,16 +703,19 @@
         <v>4</v>
       </c>
       <c r="J4" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L4" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>43633.412607152779</v>
       </c>
@@ -707,35 +725,39 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
+      <c r="D5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5</v>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H5" s="2">
         <v>5</v>
       </c>
       <c r="I5" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
         <v>3</v>
       </c>
       <c r="L5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43633.41689576389</v>
       </c>
@@ -745,26 +767,27 @@
       <c r="C6" s="4">
         <v>15</v>
       </c>
-      <c r="D6" s="4">
-        <v>2</v>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
         <v>22</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>3</v>
+      <c r="G6" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="H6" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K6" s="4">
         <v>3</v>
@@ -772,8 +795,11 @@
       <c r="L6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="M6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43633.420711400468</v>
       </c>
@@ -783,35 +809,39 @@
       <c r="C7" s="4">
         <v>30</v>
       </c>
-      <c r="D7" s="4">
-        <v>2</v>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
         <v>22</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="4">
         <v>4</v>
       </c>
       <c r="I7" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J7" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K7" s="4">
         <v>2</v>
       </c>
       <c r="L7" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>43633.428848148149</v>
       </c>
@@ -821,35 +851,39 @@
       <c r="C8" s="10">
         <v>15</v>
       </c>
-      <c r="D8" s="10">
-        <v>3</v>
+      <c r="D8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="10">
         <v>24</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="G8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L8" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M8" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>43633.43254829861</v>
       </c>
@@ -859,35 +893,39 @@
       <c r="C9" s="13">
         <v>0</v>
       </c>
-      <c r="D9" s="13">
-        <v>3</v>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="E9" s="13">
+        <v>3</v>
+      </c>
+      <c r="F9" s="13">
         <v>24</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="G9" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K9" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L9" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="M9" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>43633.436213564812</v>
       </c>
@@ -897,35 +935,39 @@
       <c r="C10" s="16">
         <v>30</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E10" s="16">
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
         <v>24</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="16">
-        <v>4</v>
+      <c r="G10" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="H10" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K10" s="16">
         <v>3</v>
       </c>
       <c r="L10" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M10" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18">
         <v>43633.44493518518</v>
       </c>
@@ -935,35 +977,39 @@
       <c r="C11" s="19">
         <v>15</v>
       </c>
-      <c r="D11" s="19">
-        <v>4</v>
+      <c r="D11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E11" s="19">
+        <v>4</v>
+      </c>
+      <c r="F11" s="19">
         <v>27</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="19">
-        <v>4</v>
+      <c r="G11" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H11" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" s="19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K11" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L11" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M11" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>43633.448915162036</v>
       </c>
@@ -973,16 +1019,17 @@
       <c r="C12" s="13">
         <v>30</v>
       </c>
-      <c r="D12" s="13">
-        <v>4</v>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E12" s="13">
+        <v>4</v>
+      </c>
+      <c r="F12" s="13">
         <v>27</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="G12" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="13">
@@ -992,16 +1039,19 @@
         <v>3</v>
       </c>
       <c r="J12" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L12" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M12" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>43633.452701226852</v>
       </c>
@@ -1011,35 +1061,39 @@
       <c r="C13" s="21">
         <v>0</v>
       </c>
-      <c r="D13" s="21">
-        <v>4</v>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="E13" s="21">
+        <v>4</v>
+      </c>
+      <c r="F13" s="21">
         <v>27</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="21">
-        <v>5</v>
+      <c r="G13" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="H13" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" s="21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L13" s="21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="M13" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18">
         <v>43633.473598009259</v>
       </c>
@@ -1049,35 +1103,39 @@
       <c r="C14" s="19">
         <v>30</v>
       </c>
-      <c r="D14" s="19">
-        <v>5</v>
+      <c r="D14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E14" s="19">
+        <v>5</v>
+      </c>
+      <c r="F14" s="19">
         <v>22</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="19">
-        <v>4</v>
+      <c r="G14" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H14" s="19">
         <v>4</v>
       </c>
       <c r="I14" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J14" s="19">
         <v>2</v>
       </c>
       <c r="K14" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>43633.477634930554</v>
       </c>
@@ -1087,35 +1145,39 @@
       <c r="C15" s="13">
         <v>15</v>
       </c>
-      <c r="D15" s="13">
-        <v>5</v>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="E15" s="13">
+        <v>5</v>
+      </c>
+      <c r="F15" s="13">
         <v>22</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="13">
+      <c r="G15" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="13">
         <v>3</v>
       </c>
       <c r="I15" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>43633.481730844913</v>
       </c>
@@ -1125,17 +1187,18 @@
       <c r="C16" s="21">
         <v>0</v>
       </c>
-      <c r="D16" s="21">
-        <v>5</v>
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="E16" s="21">
+        <v>5</v>
+      </c>
+      <c r="F16" s="21">
         <v>22</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="21">
-        <v>5</v>
+      <c r="G16" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="H16" s="21">
         <v>5</v>
@@ -1144,16 +1207,19 @@
         <v>5</v>
       </c>
       <c r="J16" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K16" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M16" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18">
         <v>43633.491056585648</v>
       </c>
@@ -1163,35 +1229,39 @@
       <c r="C17" s="19">
         <v>30</v>
       </c>
-      <c r="D17" s="19">
-        <v>6</v>
+      <c r="D17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E17" s="19">
+        <v>6</v>
+      </c>
+      <c r="F17" s="19">
         <v>24</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="19">
-        <v>5</v>
+      <c r="G17" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="H17" s="19">
         <v>5</v>
       </c>
       <c r="I17" s="19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J17" s="19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K17" s="19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L17" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M17" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22">
         <v>43633.494855868055</v>
       </c>
@@ -1201,35 +1271,39 @@
       <c r="C18" s="23">
         <v>0</v>
       </c>
-      <c r="D18" s="23">
-        <v>6</v>
+      <c r="D18" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="E18" s="23">
+        <v>6</v>
+      </c>
+      <c r="F18" s="23">
         <v>24</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="23">
-        <v>6</v>
+      <c r="G18" s="23" t="s">
+        <v>4</v>
       </c>
       <c r="H18" s="23">
         <v>6</v>
       </c>
       <c r="I18" s="23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J18" s="23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K18" s="23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L18" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M18" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>43633.498655266201</v>
       </c>
@@ -1239,35 +1313,39 @@
       <c r="C19" s="16">
         <v>15</v>
       </c>
-      <c r="D19" s="16">
-        <v>6</v>
+      <c r="D19" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E19" s="16">
+        <v>6</v>
+      </c>
+      <c r="F19" s="16">
         <v>24</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="16">
-        <v>6</v>
+      <c r="G19" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H19" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I19" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J19" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K19" s="16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L19" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="M19" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>43633.543088784718</v>
       </c>
@@ -1277,35 +1355,39 @@
       <c r="C20" s="10">
         <v>0</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E20" s="10">
         <v>7</v>
       </c>
-      <c r="E20" s="10">
+      <c r="F20" s="10">
         <v>21</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="10">
-        <v>5</v>
+      <c r="G20" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="H20" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K20" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L20" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M20" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>43633.547102048615</v>
       </c>
@@ -1315,35 +1397,39 @@
       <c r="C21" s="13">
         <v>15</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
         <v>7</v>
       </c>
-      <c r="E21" s="13">
+      <c r="F21" s="13">
         <v>21</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="13">
+      <c r="G21" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
       </c>
       <c r="J21" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K21" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L21" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="M21" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>43633.55106489583</v>
       </c>
@@ -1353,35 +1439,39 @@
       <c r="C22" s="16">
         <v>30</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
         <v>7</v>
       </c>
-      <c r="E22" s="16">
+      <c r="F22" s="16">
         <v>21</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="16">
-        <v>2</v>
+      <c r="G22" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H22" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="16">
         <v>1</v>
       </c>
       <c r="J22" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K22" s="16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L22" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="M22" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>43633.56562115741</v>
       </c>
@@ -1391,35 +1481,39 @@
       <c r="C23" s="10">
         <v>0</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E23" s="10">
         <v>8</v>
       </c>
-      <c r="E23" s="10">
+      <c r="F23" s="10">
         <v>25</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="10">
-        <v>4</v>
+      <c r="G23" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="H23" s="10">
         <v>4</v>
       </c>
       <c r="I23" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J23" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K23" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="M23" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>43633.569439791667</v>
       </c>
@@ -1429,16 +1523,17 @@
       <c r="C24" s="13">
         <v>30</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
         <v>8</v>
       </c>
-      <c r="E24" s="13">
+      <c r="F24" s="13">
         <v>25</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="13">
+      <c r="G24" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="13">
@@ -1448,16 +1543,19 @@
         <v>3</v>
       </c>
       <c r="J24" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L24" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M24" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <v>43633.573091435188</v>
       </c>
@@ -1467,35 +1565,39 @@
       <c r="C25" s="16">
         <v>15</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E25" s="16">
         <v>8</v>
       </c>
-      <c r="E25" s="16">
+      <c r="F25" s="16">
         <v>25</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="16">
-        <v>5</v>
+      <c r="G25" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="H25" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25" s="16">
         <v>4</v>
       </c>
       <c r="J25" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K25" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="M25" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18">
         <v>43633.621917488425</v>
       </c>
@@ -1505,35 +1607,39 @@
       <c r="C26" s="19">
         <v>15</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E26" s="19">
         <v>9</v>
       </c>
-      <c r="E26" s="19">
+      <c r="F26" s="19">
         <v>24</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="19">
+      <c r="G26" s="19" t="s">
         <v>4</v>
       </c>
       <c r="H26" s="19">
         <v>4</v>
       </c>
       <c r="I26" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J26" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L26" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="M26" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="22">
         <v>43633.626015983798</v>
       </c>
@@ -1543,17 +1649,18 @@
       <c r="C27" s="23">
         <v>0</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E27" s="23">
         <v>9</v>
       </c>
-      <c r="E27" s="23">
+      <c r="F27" s="23">
         <v>24</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="23">
-        <v>5</v>
+      <c r="G27" s="23" t="s">
+        <v>4</v>
       </c>
       <c r="H27" s="23">
         <v>5</v>
@@ -1562,16 +1669,19 @@
         <v>5</v>
       </c>
       <c r="J27" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K27" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L27" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M27" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>43633.630061898148</v>
       </c>
@@ -1581,35 +1691,39 @@
       <c r="C28" s="16">
         <v>30</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="16">
         <v>9</v>
       </c>
-      <c r="E28" s="16">
+      <c r="F28" s="16">
         <v>24</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="16">
-        <v>2</v>
+      <c r="G28" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H28" s="16">
         <v>2</v>
       </c>
       <c r="I28" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K28" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="M28" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="18">
         <v>43633.635984166671</v>
       </c>
@@ -1619,17 +1733,18 @@
       <c r="C29" s="19">
         <v>15</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E29" s="19">
         <v>10</v>
       </c>
-      <c r="E29" s="19">
+      <c r="F29" s="19">
         <v>32</v>
       </c>
-      <c r="F29" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="19">
-        <v>2</v>
+      <c r="G29" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H29" s="19">
         <v>2</v>
@@ -1638,16 +1753,19 @@
         <v>2</v>
       </c>
       <c r="J29" s="19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K29" s="19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L29" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M29" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>43633.639922939816</v>
       </c>
@@ -1657,17 +1775,18 @@
       <c r="C30" s="13">
         <v>30</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="13">
         <v>10</v>
       </c>
-      <c r="E30" s="13">
+      <c r="F30" s="13">
         <v>32</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="13">
-        <v>2</v>
+      <c r="G30" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="H30" s="13">
         <v>2</v>
@@ -1676,16 +1795,19 @@
         <v>2</v>
       </c>
       <c r="J30" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K30" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L30" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="M30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>43633.644036076388</v>
       </c>
@@ -1695,35 +1817,39 @@
       <c r="C31" s="21">
         <v>0</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E31" s="21">
         <v>10</v>
       </c>
-      <c r="E31" s="21">
+      <c r="F31" s="21">
         <v>32</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="21">
+      <c r="G31" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H31" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31" s="21">
         <v>2</v>
       </c>
       <c r="J31" s="21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K31" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L31" s="21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="M31" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="18">
         <v>43633.656176157412</v>
       </c>
@@ -1733,35 +1859,39 @@
       <c r="C32" s="19">
         <v>30</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E32" s="19">
         <v>11</v>
       </c>
-      <c r="E32" s="19">
+      <c r="F32" s="19">
         <v>28</v>
       </c>
-      <c r="F32" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="19">
-        <v>2</v>
+      <c r="G32" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="H32" s="19">
         <v>2</v>
       </c>
       <c r="I32" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K32" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L32" s="19">
+        <v>4</v>
+      </c>
+      <c r="M32" s="19">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="22">
         <v>43633.660050752311</v>
       </c>
@@ -1771,35 +1901,39 @@
       <c r="C33" s="23">
         <v>0</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E33" s="23">
         <v>11</v>
       </c>
-      <c r="E33" s="23">
+      <c r="F33" s="23">
         <v>28</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="23">
-        <v>5</v>
+      <c r="G33" s="23" t="s">
+        <v>4</v>
       </c>
       <c r="H33" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I33" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J33" s="23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K33" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L33" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M33" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>43633.663931643518</v>
       </c>
@@ -1809,35 +1943,39 @@
       <c r="C34" s="16">
         <v>15</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="16">
         <v>11</v>
       </c>
-      <c r="E34" s="16">
+      <c r="F34" s="16">
         <v>28</v>
       </c>
-      <c r="F34" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="16">
-        <v>3</v>
+      <c r="G34" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H34" s="16">
         <v>3</v>
       </c>
       <c r="I34" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J34" s="16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K34" s="16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L34" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M34" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="18">
         <v>43633.671505023143</v>
       </c>
@@ -1847,26 +1985,27 @@
       <c r="C35" s="19">
         <v>30</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E35" s="19">
         <v>12</v>
       </c>
-      <c r="E35" s="19">
+      <c r="F35" s="19">
         <v>29</v>
       </c>
-      <c r="F35" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="19">
-        <v>5</v>
+      <c r="G35" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H35" s="19">
         <v>5</v>
       </c>
       <c r="I35" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J35" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K35" s="19">
         <v>4</v>
@@ -1874,8 +2013,11 @@
       <c r="L35" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M35" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>43633.675077256943</v>
       </c>
@@ -1885,35 +2027,39 @@
       <c r="C36" s="13">
         <v>15</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36" s="13">
         <v>12</v>
       </c>
-      <c r="E36" s="13">
+      <c r="F36" s="13">
         <v>29</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="13">
-        <v>6</v>
+      <c r="G36" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="H36" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I36" s="13">
         <v>5</v>
       </c>
       <c r="J36" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K36" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L36" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="M36" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>43633.678634583332</v>
       </c>
@@ -1923,35 +2069,39 @@
       <c r="C37" s="21">
         <v>0</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E37" s="21">
         <v>12</v>
       </c>
-      <c r="E37" s="21">
+      <c r="F37" s="21">
         <v>29</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37" s="21">
-        <v>5</v>
+      <c r="G37" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="H37" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I37" s="21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J37" s="21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K37" s="21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L37" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M37" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9">
         <v>43633.687255833334</v>
       </c>
@@ -1961,35 +2111,39 @@
       <c r="C38" s="10">
         <v>0</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E38" s="10">
         <v>13</v>
       </c>
-      <c r="E38" s="10">
+      <c r="F38" s="10">
         <v>28</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="10">
-        <v>5</v>
+      <c r="G38" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="H38" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I38" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J38" s="10">
+        <v>1</v>
+      </c>
+      <c r="K38" s="10">
         <v>7</v>
       </c>
-      <c r="K38" s="10">
-        <v>5</v>
-      </c>
       <c r="L38" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="M38" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>43633.690993599535</v>
       </c>
@@ -1999,35 +2153,39 @@
       <c r="C39" s="13">
         <v>15</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="13">
         <v>13</v>
       </c>
-      <c r="E39" s="13">
+      <c r="F39" s="13">
         <v>28</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="13">
-        <v>5</v>
+      <c r="G39" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="H39" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I39" s="13">
         <v>1</v>
       </c>
       <c r="J39" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K39" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L39" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="M39" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>43633.69486265046</v>
       </c>
@@ -2037,35 +2195,39 @@
       <c r="C40" s="16">
         <v>30</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="16">
         <v>13</v>
       </c>
-      <c r="E40" s="16">
+      <c r="F40" s="16">
         <v>28</v>
       </c>
-      <c r="F40" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="16">
-        <v>5</v>
+      <c r="G40" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H40" s="16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I40" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40" s="16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K40" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L40" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M40" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="9">
         <v>43634.42713611111</v>
       </c>
@@ -2075,35 +2237,39 @@
       <c r="C41" s="10">
         <v>0</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E41" s="10">
         <v>14</v>
       </c>
-      <c r="E41" s="10">
+      <c r="F41" s="10">
         <v>23</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="10">
-        <v>4</v>
+      <c r="G41" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="H41" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J41" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K41" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L41" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="M41" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>43634.430535613428</v>
       </c>
@@ -2113,35 +2279,39 @@
       <c r="C42" s="13">
         <v>30</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D42" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="13">
         <v>14</v>
       </c>
-      <c r="E42" s="13">
+      <c r="F42" s="13">
         <v>23</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" s="13">
-        <v>4</v>
+      <c r="G42" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="H42" s="13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I42" s="13">
+        <v>6</v>
+      </c>
+      <c r="J42" s="13">
         <v>7</v>
       </c>
-      <c r="J42" s="13">
-        <v>4</v>
-      </c>
       <c r="K42" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L42" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M42" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <v>43634.433871006942</v>
       </c>
@@ -2151,35 +2321,39 @@
       <c r="C43" s="16">
         <v>15</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E43" s="16">
         <v>14</v>
       </c>
-      <c r="E43" s="16">
+      <c r="F43" s="16">
         <v>23</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" s="16">
-        <v>4</v>
+      <c r="G43" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="H43" s="16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I43" s="16">
+        <v>6</v>
+      </c>
+      <c r="J43" s="16">
         <v>7</v>
       </c>
-      <c r="J43" s="16">
-        <v>4</v>
-      </c>
       <c r="K43" s="16">
         <v>4</v>
       </c>
       <c r="L43" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M43" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>43634.441357303236</v>
       </c>
@@ -2189,35 +2363,39 @@
       <c r="C44" s="19">
         <v>15</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D44" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E44" s="19">
         <v>15</v>
       </c>
-      <c r="E44" s="19">
+      <c r="F44" s="19">
         <v>21</v>
       </c>
-      <c r="F44" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" s="19">
-        <v>4</v>
+      <c r="G44" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H44" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I44" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J44" s="19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K44" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L44" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M44" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="22">
         <v>43634.445045555556</v>
       </c>
@@ -2227,35 +2405,39 @@
       <c r="C45" s="23">
         <v>0</v>
       </c>
-      <c r="D45" s="23">
+      <c r="D45" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E45" s="23">
         <v>15</v>
       </c>
-      <c r="E45" s="23">
+      <c r="F45" s="23">
         <v>21</v>
       </c>
-      <c r="F45" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="23">
-        <v>4</v>
+      <c r="G45" s="23" t="s">
+        <v>3</v>
       </c>
       <c r="H45" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I45" s="23">
         <v>3</v>
       </c>
       <c r="J45" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K45" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L45" s="23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M45" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>43634.448615891204</v>
       </c>
@@ -2265,35 +2447,39 @@
       <c r="C46" s="16">
         <v>30</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="16">
         <v>15</v>
       </c>
-      <c r="E46" s="16">
+      <c r="F46" s="16">
         <v>21</v>
       </c>
-      <c r="F46" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="16">
-        <v>4</v>
+      <c r="G46" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="H46" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I46" s="16">
         <v>3</v>
       </c>
       <c r="J46" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K46" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L46" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M46" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>43634.456436817127</v>
       </c>
@@ -2303,35 +2489,39 @@
       <c r="C47" s="19">
         <v>15</v>
       </c>
-      <c r="D47" s="19">
+      <c r="D47" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E47" s="19">
         <v>16</v>
       </c>
-      <c r="E47" s="19">
+      <c r="F47" s="19">
         <v>23</v>
       </c>
-      <c r="F47" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G47" s="19">
+      <c r="G47" s="19" t="s">
         <v>4</v>
       </c>
       <c r="H47" s="19">
         <v>4</v>
       </c>
       <c r="I47" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J47" s="19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K47" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L47" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M47" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>43634.460279965278</v>
       </c>
@@ -2341,35 +2531,39 @@
       <c r="C48" s="13">
         <v>30</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="13">
         <v>16</v>
       </c>
-      <c r="E48" s="13">
+      <c r="F48" s="13">
         <v>23</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="13">
+      <c r="G48" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H48" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I48" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J48" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K48" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L48" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="M48" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>43634.464040173611</v>
       </c>
@@ -2379,35 +2573,39 @@
       <c r="C49" s="21">
         <v>0</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E49" s="21">
         <v>16</v>
       </c>
-      <c r="E49" s="21">
+      <c r="F49" s="21">
         <v>23</v>
       </c>
-      <c r="F49" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G49" s="21">
+      <c r="G49" s="21" t="s">
         <v>4</v>
       </c>
       <c r="H49" s="21">
         <v>4</v>
       </c>
       <c r="I49" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J49" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K49" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L49" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M49" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="18">
         <v>43634.472191168985</v>
       </c>
@@ -2417,35 +2615,39 @@
       <c r="C50" s="19">
         <v>30</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D50" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E50" s="19">
         <v>17</v>
       </c>
-      <c r="E50" s="19">
+      <c r="F50" s="19">
         <v>21</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" s="19">
-        <v>2</v>
+      <c r="G50" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H50" s="19">
         <v>2</v>
       </c>
       <c r="I50" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J50" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L50" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="M50" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="22">
         <v>43634.476160416671</v>
       </c>
@@ -2455,35 +2657,39 @@
       <c r="C51" s="23">
         <v>0</v>
       </c>
-      <c r="D51" s="23">
+      <c r="D51" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E51" s="23">
         <v>17</v>
       </c>
-      <c r="E51" s="23">
+      <c r="F51" s="23">
         <v>21</v>
       </c>
-      <c r="F51" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G51" s="23">
-        <v>4</v>
+      <c r="G51" s="23" t="s">
+        <v>3</v>
       </c>
       <c r="H51" s="23">
         <v>4</v>
       </c>
       <c r="I51" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J51" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K51" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L51" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="M51" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
         <v>43634.479981168981</v>
       </c>
@@ -2493,35 +2699,39 @@
       <c r="C52" s="16">
         <v>15</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="16">
         <v>17</v>
       </c>
-      <c r="E52" s="16">
+      <c r="F52" s="16">
         <v>21</v>
       </c>
-      <c r="F52" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G52" s="16">
+      <c r="G52" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H52" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I52" s="16">
         <v>4</v>
       </c>
       <c r="J52" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K52" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L52" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="M52" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="18">
         <v>43634.518777372687</v>
       </c>
@@ -2531,35 +2741,39 @@
       <c r="C53" s="19">
         <v>30</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E53" s="19">
         <v>18</v>
       </c>
-      <c r="E53" s="19">
+      <c r="F53" s="19">
         <v>25</v>
       </c>
-      <c r="F53" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G53" s="19">
-        <v>5</v>
+      <c r="G53" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="H53" s="19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J53" s="19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K53" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L53" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M53" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="12">
         <v>43634.522951238425</v>
       </c>
@@ -2569,35 +2783,39 @@
       <c r="C54" s="13">
         <v>15</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E54" s="13">
         <v>18</v>
       </c>
-      <c r="E54" s="13">
+      <c r="F54" s="13">
         <v>25</v>
       </c>
-      <c r="F54" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G54" s="13">
+      <c r="G54" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H54" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I54" s="13">
         <v>2</v>
       </c>
       <c r="J54" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K54" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L54" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="M54" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>43634.526760381945</v>
       </c>
@@ -2607,35 +2825,39 @@
       <c r="C55" s="21">
         <v>0</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E55" s="21">
         <v>18</v>
       </c>
-      <c r="E55" s="21">
+      <c r="F55" s="21">
         <v>25</v>
       </c>
-      <c r="F55" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" s="21">
-        <v>6</v>
+      <c r="G55" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="H55" s="21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I55" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J55" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K55" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L55" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M55" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="9">
         <v>43634.536091597227</v>
       </c>
@@ -2645,26 +2867,27 @@
       <c r="C56" s="10">
         <v>0</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E56" s="10">
         <v>19</v>
       </c>
-      <c r="E56" s="10">
+      <c r="F56" s="10">
         <v>26</v>
       </c>
-      <c r="F56" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G56" s="10">
-        <v>5</v>
+      <c r="G56" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="H56" s="10">
         <v>5</v>
       </c>
       <c r="I56" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J56" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K56" s="10">
         <v>2</v>
@@ -2672,8 +2895,11 @@
       <c r="L56" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M56" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="12">
         <v>43634.53982633102</v>
       </c>
@@ -2683,35 +2909,39 @@
       <c r="C57" s="13">
         <v>15</v>
       </c>
-      <c r="D57" s="13">
+      <c r="D57" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="13">
         <v>19</v>
       </c>
-      <c r="E57" s="13">
+      <c r="F57" s="13">
         <v>26</v>
       </c>
-      <c r="F57" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G57" s="13">
+      <c r="G57" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H57" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I57" s="13">
         <v>5</v>
       </c>
       <c r="J57" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K57" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L57" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="M57" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15">
         <v>43634.543295636569</v>
       </c>
@@ -2721,35 +2951,39 @@
       <c r="C58" s="16">
         <v>30</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D58" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="16">
         <v>19</v>
       </c>
-      <c r="E58" s="16">
+      <c r="F58" s="16">
         <v>26</v>
       </c>
-      <c r="F58" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G58" s="16">
-        <v>2</v>
+      <c r="G58" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H58" s="16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I58" s="16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J58" s="16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K58" s="16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L58" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M58" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="9">
         <v>43634.554000891207</v>
       </c>
@@ -2759,35 +2993,39 @@
       <c r="C59" s="10">
         <v>0</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E59" s="10">
         <v>20</v>
       </c>
-      <c r="E59" s="10">
+      <c r="F59" s="10">
         <v>32</v>
       </c>
-      <c r="F59" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G59" s="10">
+      <c r="G59" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H59" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I59" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J59" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K59" s="10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L59" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="M59" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="12">
         <v>43634.557719328703</v>
       </c>
@@ -2797,35 +3035,39 @@
       <c r="C60" s="13">
         <v>30</v>
       </c>
-      <c r="D60" s="13">
+      <c r="D60" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="13">
         <v>20</v>
       </c>
-      <c r="E60" s="13">
+      <c r="F60" s="13">
         <v>32</v>
       </c>
-      <c r="F60" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G60" s="13">
-        <v>2</v>
+      <c r="G60" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="H60" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I60" s="13">
         <v>3</v>
       </c>
       <c r="J60" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K60" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L60" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="M60" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
         <v>43634.561903645837</v>
       </c>
@@ -2835,17 +3077,18 @@
       <c r="C61" s="16">
         <v>15</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E61" s="16">
         <v>20</v>
       </c>
-      <c r="E61" s="16">
+      <c r="F61" s="16">
         <v>32</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G61" s="16">
-        <v>2</v>
+      <c r="G61" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H61" s="16">
         <v>2</v>
@@ -2854,17 +3097,20 @@
         <v>2</v>
       </c>
       <c r="J61" s="16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K61" s="16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L61" s="16">
+        <v>4</v>
+      </c>
+      <c r="M61" s="16">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L61">
+  <sortState ref="A2:M61">
     <sortCondition ref="A2:A61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>